<commit_message>
changed type of calculations, potentially became slower
</commit_message>
<xml_diff>
--- a/public/sheets/finCalculatorA.xlsx
+++ b/public/sheets/finCalculatorA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\makar\Desktop\Calcscout24\Website creation\calcscout\public\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FEF25BC-3783-4F0C-A1D1-35CE597B0D49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00668D7E-05F7-49DE-98D6-5DC8AC0E5A18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="23310" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,20 +16,20 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="inputAnnualInterest">Sheet1!$C$3</definedName>
-    <definedName name="inputLoanAmount">Sheet1!$C$2</definedName>
-    <definedName name="inputMonthlyPayment">Sheet1!$C$5</definedName>
-    <definedName name="inputNumberOfPeriods">Sheet1!$C$4</definedName>
-    <definedName name="outputEffectiveInterestC2">Sheet1!$C$25</definedName>
-    <definedName name="outputInterestPerYearC1">Sheet1!$C$17</definedName>
-    <definedName name="outputMonthlyPaymentC1">Sheet1!$C$14</definedName>
-    <definedName name="outputPrincipalPerYearC1">Sheet1!$C$16</definedName>
-    <definedName name="outputTotalInterestRepaidC1">Sheet1!$C$11</definedName>
-    <definedName name="outputTotalInterestRepaidC2">Sheet1!$C$22</definedName>
-    <definedName name="outputTotalPrincipalInterestRepaidC1">Sheet1!$C$12</definedName>
-    <definedName name="outputTotalPrincipalInterestRepaidC2">Sheet1!$C$23</definedName>
-    <definedName name="outputTotalPrincipalRepaidC1">Sheet1!$C$10</definedName>
-    <definedName name="outputTotalPrincipalRepaidC2">Sheet1!$C$21</definedName>
+    <definedName name="inputAnnualInterest">Sheet1!$D$4</definedName>
+    <definedName name="inputLoanAmount">Sheet1!$D$3</definedName>
+    <definedName name="inputMonthlyPayment">Sheet1!$D$6</definedName>
+    <definedName name="inputNumberOfPeriods">Sheet1!$D$5</definedName>
+    <definedName name="outputEffectiveInterestC2">Sheet1!$D$26</definedName>
+    <definedName name="outputInterestPerYearC1">Sheet1!$D$18</definedName>
+    <definedName name="outputMonthlyPaymentC1">Sheet1!$D$15</definedName>
+    <definedName name="outputPrincipalPerYearC1">Sheet1!$D$17</definedName>
+    <definedName name="outputTotalInterestRepaidC1">Sheet1!$D$12</definedName>
+    <definedName name="outputTotalInterestRepaidC2">Sheet1!$D$23</definedName>
+    <definedName name="outputTotalPrincipalInterestRepaidC1">Sheet1!$D$13</definedName>
+    <definedName name="outputTotalPrincipalInterestRepaidC2">Sheet1!$D$24</definedName>
+    <definedName name="outputTotalPrincipalRepaidC1">Sheet1!$D$11</definedName>
+    <definedName name="outputTotalPrincipalRepaidC2">Sheet1!$D$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>Inputs</t>
   </si>
@@ -143,6 +143,39 @@
   </si>
   <si>
     <t>outputTotalPrincipalRepaidC2</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>Year 1</t>
+  </si>
+  <si>
+    <t>Year 2</t>
+  </si>
+  <si>
+    <t>Year 3</t>
+  </si>
+  <si>
+    <t>Year 4</t>
+  </si>
+  <si>
+    <t>Year 5</t>
+  </si>
+  <si>
+    <t>Year 6</t>
+  </si>
+  <si>
+    <t>Year 7</t>
+  </si>
+  <si>
+    <t>Year 8</t>
+  </si>
+  <si>
+    <t>Year 9</t>
+  </si>
+  <si>
+    <t>Year 10</t>
   </si>
 </sst>
 </file>
@@ -154,7 +187,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,6 +234,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -534,288 +573,526 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
         <v>3</v>
       </c>
-      <c r="C2" s="9">
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>7</v>
+      </c>
+      <c r="H1">
+        <v>8</v>
+      </c>
+      <c r="I1">
+        <v>9</v>
+      </c>
+      <c r="J1">
+        <v>10</v>
+      </c>
+      <c r="K1">
+        <v>11</v>
+      </c>
+      <c r="L1">
+        <v>12</v>
+      </c>
+      <c r="M1">
+        <v>13</v>
+      </c>
+      <c r="N1">
+        <v>14</v>
+      </c>
+      <c r="O1">
+        <v>15</v>
+      </c>
+      <c r="P1">
+        <v>16</v>
+      </c>
+      <c r="Q1">
+        <v>17</v>
+      </c>
+      <c r="R1">
+        <v>18</v>
+      </c>
+      <c r="S1">
+        <v>19</v>
+      </c>
+      <c r="T1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="9">
         <v>10000</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="10">
+      <c r="D4" s="10">
         <v>3.9899999999999998E-2</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="9">
         <v>60</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E5" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D6" s="1">
         <v>200</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
         <v>6</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="3">
-        <f>C2</f>
+      <c r="D11" s="3">
+        <f>D3</f>
         <v>10000</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="E11" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="4">
-        <f>-CUMIPMT($C$3/12,$C$4,$C$2,1,$C$4,0)</f>
+      <c r="D12" s="4">
+        <f>-CUMIPMT($D$4/12,$D$5,$D$3,1,$D$5,0)</f>
         <v>1047.2057883855614</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="E12" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="4">
-        <f>C10+C11</f>
+      <c r="D13" s="4">
+        <f>D11+D12</f>
         <v>11047.205788385561</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="E13" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="C14" s="5">
-        <f>-PMT($C$3/12,$C$4,$C$2)</f>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="5">
+        <f>-PMT($D$4/12,$D$5,$D$3)</f>
         <v>184.12009647309273</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="E15" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="4">
-        <f>C10/C4*12</f>
+      <c r="D17" s="4">
+        <f>D11/D5*12</f>
         <v>2000</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="E17" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="4">
-        <f>C11/C4*12</f>
+      <c r="D18" s="4">
+        <f>D12/D5*12</f>
         <v>209.44115767711227</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="E18" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
         <v>6</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="3">
-        <f>C2</f>
+      <c r="D22" s="3">
+        <f>D3</f>
         <v>10000</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="E22" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="4">
-        <f>C23-C21</f>
+      <c r="D23" s="4">
+        <f>D24-D22</f>
         <v>2000</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="E23" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="4">
-        <f>C5*C4</f>
+      <c r="D24" s="4">
+        <f>D6*D5</f>
         <v>12000</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="E24" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="7">
-        <f>RATE($C$4,-$C$5,$C$2)*12</f>
+      <c r="D26" s="7">
+        <f>RATE($D$5,-$D$6,$D$3)*12</f>
         <v>7.4200957935045442E-2</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="E26" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="33" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="34" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="35" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="36" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="37" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="38" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="39" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="40" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="41" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="42" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="43" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="44" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="45" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="46" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="47" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="48" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="49" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="50" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="51" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="52" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="53" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="54" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="55" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="56" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="57" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="58" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="59" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="60" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="61" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="62" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="63" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="64" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" t="s">
+        <v>35</v>
+      </c>
+      <c r="F30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G30" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30" t="s">
+        <v>38</v>
+      </c>
+      <c r="I30" t="s">
+        <v>39</v>
+      </c>
+      <c r="J30" t="s">
+        <v>40</v>
+      </c>
+      <c r="K30" t="s">
+        <v>41</v>
+      </c>
+      <c r="L30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
deleted names from excel, dynamic years array
</commit_message>
<xml_diff>
--- a/public/sheets/finCalculatorA.xlsx
+++ b/public/sheets/finCalculatorA.xlsx
@@ -8,29 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\makar\Desktop\Calcscout24\Website creation\calcscout\public\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00668D7E-05F7-49DE-98D6-5DC8AC0E5A18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE003D31-2666-4522-96A9-C0F74F8D87EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="23310" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="inputAnnualInterest">Sheet1!$D$4</definedName>
-    <definedName name="inputLoanAmount">Sheet1!$D$3</definedName>
-    <definedName name="inputMonthlyPayment">Sheet1!$D$6</definedName>
-    <definedName name="inputNumberOfPeriods">Sheet1!$D$5</definedName>
-    <definedName name="outputEffectiveInterestC2">Sheet1!$D$26</definedName>
-    <definedName name="outputInterestPerYearC1">Sheet1!$D$18</definedName>
-    <definedName name="outputMonthlyPaymentC1">Sheet1!$D$15</definedName>
-    <definedName name="outputPrincipalPerYearC1">Sheet1!$D$17</definedName>
-    <definedName name="outputTotalInterestRepaidC1">Sheet1!$D$12</definedName>
-    <definedName name="outputTotalInterestRepaidC2">Sheet1!$D$23</definedName>
-    <definedName name="outputTotalPrincipalInterestRepaidC1">Sheet1!$D$13</definedName>
-    <definedName name="outputTotalPrincipalInterestRepaidC2">Sheet1!$D$24</definedName>
-    <definedName name="outputTotalPrincipalRepaidC1">Sheet1!$D$11</definedName>
-    <definedName name="outputTotalPrincipalRepaidC2">Sheet1!$D$22</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>Inputs</t>
   </si>
@@ -145,9 +129,6 @@
     <t>outputTotalPrincipalRepaidC2</t>
   </si>
   <si>
-    <t>Years</t>
-  </si>
-  <si>
     <t>Year 1</t>
   </si>
   <si>
@@ -176,6 +157,30 @@
   </si>
   <si>
     <t>Year 10</t>
+  </si>
+  <si>
+    <t>Start Num</t>
+  </si>
+  <si>
+    <t>End Num</t>
+  </si>
+  <si>
+    <t>Flag</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Period name</t>
+  </si>
+  <si>
+    <t>Supporting</t>
+  </si>
+  <si>
+    <t>Full years</t>
+  </si>
+  <si>
+    <t>Interest payments</t>
   </si>
 </sst>
 </file>
@@ -278,7 +283,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -292,6 +297,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -575,16 +586,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="1" max="3" width="9.140625" outlineLevel="1"/>
+    <col min="4" max="4" width="31.42578125" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -592,65 +609,71 @@
         <v>1</v>
       </c>
       <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
         <v>3</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>4</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <v>5</v>
       </c>
-      <c r="F1">
+      <c r="G1">
         <v>6</v>
       </c>
-      <c r="G1">
+      <c r="H1">
         <v>7</v>
       </c>
-      <c r="H1">
+      <c r="I1">
         <v>8</v>
       </c>
-      <c r="I1">
+      <c r="J1">
         <v>9</v>
       </c>
-      <c r="J1">
+      <c r="K1">
         <v>10</v>
       </c>
-      <c r="K1">
+      <c r="L1">
         <v>11</v>
       </c>
-      <c r="L1">
+      <c r="M1">
         <v>12</v>
       </c>
-      <c r="M1">
+      <c r="N1">
         <v>13</v>
       </c>
-      <c r="N1">
+      <c r="O1">
         <v>14</v>
       </c>
-      <c r="O1">
+      <c r="P1">
         <v>15</v>
       </c>
-      <c r="P1">
+      <c r="Q1">
         <v>16</v>
       </c>
-      <c r="Q1">
+      <c r="R1">
         <v>17</v>
       </c>
-      <c r="R1">
+      <c r="S1">
         <v>18</v>
       </c>
-      <c r="S1">
+      <c r="T1">
         <v>19</v>
-      </c>
-      <c r="T1">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>0</v>
       </c>
     </row>
@@ -658,13 +681,13 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="9">
+      <c r="F3" s="9">
         <v>10000</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="G3" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -672,13 +695,13 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="10">
+      <c r="F4" s="10">
         <v>3.9899999999999998E-2</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -686,13 +709,13 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="9">
+      <c r="F5" s="9">
         <v>60</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -700,13 +723,13 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="1">
+      <c r="F6" s="1">
         <v>200</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>21</v>
       </c>
     </row>
@@ -719,7 +742,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>1</v>
       </c>
     </row>
@@ -727,7 +750,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>12</v>
       </c>
     </row>
@@ -735,10 +758,10 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>6</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>14</v>
       </c>
     </row>
@@ -746,14 +769,14 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="3">
-        <f>D3</f>
+      <c r="F11" s="3">
+        <f>F3</f>
         <v>10000</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="G11" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -761,14 +784,14 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="4">
-        <f>-CUMIPMT($D$4/12,$D$5,$D$3,1,$D$5,0)</f>
+      <c r="F12" s="4">
+        <f>-CUMIPMT($F$4/12,$F$5,$F$3,1,$F$5,0)</f>
         <v>1047.2057883855614</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="G12" s="8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -776,14 +799,14 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="4">
-        <f>D11+D12</f>
+      <c r="F13" s="4">
+        <f>F11+F12</f>
         <v>11047.205788385561</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="G13" s="8" t="s">
         <v>24</v>
       </c>
     </row>
@@ -791,21 +814,21 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="5">
-        <f>-PMT($D$4/12,$D$5,$D$3)</f>
+      <c r="F15" s="5">
+        <f>-PMT($F$4/12,$F$5,$F$3)</f>
         <v>184.12009647309273</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="G15" s="8" t="s">
         <v>25</v>
       </c>
     </row>
@@ -813,270 +836,366 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="4">
-        <f>D11/D5*12</f>
+      <c r="F17" s="4">
+        <f>F11/F5*12</f>
         <v>2000</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="G17" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="4">
-        <f>D12/D5*12</f>
+      <c r="F18" s="4">
+        <f>F12/F5*12</f>
         <v>209.44115767711227</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="G18" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E21" t="s">
         <v>6</v>
       </c>
-      <c r="E21" t="s">
+      <c r="G21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="3">
-        <f>D3</f>
+      <c r="F22" s="3">
+        <f>F3</f>
         <v>10000</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="G22" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="4">
-        <f>D24-D22</f>
+      <c r="F23" s="4">
+        <f>F24-F22</f>
         <v>2000</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="G23" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="4">
-        <f>D6*D5</f>
+      <c r="F24" s="4">
+        <f>F6*F5</f>
         <v>12000</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="G24" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="7">
-        <f>RATE($D$5,-$D$6,$D$3)*12</f>
+      <c r="F26" s="7">
+        <f>RATE($F$5,-$F$6,$F$3)*12</f>
         <v>7.4200957935045442E-2</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="G26" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F28">
+        <f>ROUNDUP(F5/12,0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E30" t="s">
-        <v>35</v>
-      </c>
-      <c r="F30" t="s">
-        <v>36</v>
-      </c>
-      <c r="G30" t="s">
-        <v>37</v>
-      </c>
-      <c r="H30" t="s">
-        <v>38</v>
-      </c>
-      <c r="I30" t="s">
-        <v>39</v>
-      </c>
-      <c r="J30" t="s">
-        <v>40</v>
-      </c>
-      <c r="K30" t="s">
-        <v>41</v>
-      </c>
-      <c r="L30" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D30" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" s="11">
+        <v>1</v>
+      </c>
+      <c r="F31" s="11">
+        <v>2</v>
+      </c>
+      <c r="G31" s="11">
+        <v>3</v>
+      </c>
+      <c r="H31" s="11">
+        <v>4</v>
+      </c>
+      <c r="I31" s="11">
+        <v>5</v>
+      </c>
+      <c r="J31" s="11">
+        <v>6</v>
+      </c>
+      <c r="K31" s="11">
+        <v>7</v>
+      </c>
+      <c r="L31" s="11">
+        <v>8</v>
+      </c>
+      <c r="M31" s="11">
+        <v>9</v>
+      </c>
+      <c r="N31" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <f>B32+SUM(E33:N33)</f>
+        <v>9</v>
+      </c>
+      <c r="D32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="K32" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="L32" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="M32" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N32" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" s="11">
+        <f>(E31&lt;=$F$28)*1</f>
+        <v>1</v>
+      </c>
+      <c r="F33" s="11">
+        <f t="shared" ref="F33:N33" si="0">(F31&lt;=$F$28)*1</f>
+        <v>1</v>
+      </c>
+      <c r="G33" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H33" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I33" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J33" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K33" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L33" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M33" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N33" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1094,6 +1213,6 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>